<commit_message>
Fire Tower Design Base
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Tower.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Tower.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16686D1F-533C-4B18-9E69-B656DED28AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A76F45F-7A47-477A-AE48-414CB55AD1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26520" yWindow="5820" windowWidth="19485" windowHeight="12165" activeTab="2" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-24615" yWindow="6975" windowWidth="23850" windowHeight="12165" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="FIRE" sheetId="5" r:id="rId1"/>
@@ -592,9 +592,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53B544D-229D-4A5B-BFF8-79DA3F65400C}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -660,7 +660,7 @@
         <v>2.5</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
         <v>0.1</v>
@@ -696,7 +696,7 @@
         <v>2.5</v>
       </c>
       <c r="F3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <v>0.1</v>
@@ -732,7 +732,7 @@
         <v>2.5</v>
       </c>
       <c r="F4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
         <v>0.1</v>
@@ -771,7 +771,7 @@
         <v>2.5</v>
       </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
         <v>0.1</v>
@@ -810,7 +810,7 @@
         <v>2.5</v>
       </c>
       <c r="F6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1">
         <v>0.1</v>
@@ -846,7 +846,7 @@
         <v>2.5</v>
       </c>
       <c r="F7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1">
         <v>0.1</v>
@@ -882,13 +882,13 @@
         <v>2.5</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H8" s="1">
-        <v>0.2</v>
+        <v>0.32</v>
       </c>
       <c r="J8" s="1" t="str">
         <f t="shared" si="0"/>
@@ -918,13 +918,13 @@
         <v>2.5</v>
       </c>
       <c r="F9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H9" s="1">
-        <v>0.2</v>
+        <v>0.32</v>
       </c>
       <c r="J9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -954,13 +954,13 @@
         <v>2.5</v>
       </c>
       <c r="F10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H10" s="1">
-        <v>0.2</v>
+        <v>0.32</v>
       </c>
       <c r="J10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -990,13 +990,13 @@
         <v>2.5</v>
       </c>
       <c r="F11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H11" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1026,13 +1026,13 @@
         <v>2.5</v>
       </c>
       <c r="F12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H12" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1062,13 +1062,13 @@
         <v>2.5</v>
       </c>
       <c r="F13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H13" s="1">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="J13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1098,13 +1098,13 @@
         <v>2.5</v>
       </c>
       <c r="F14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="H14" s="1">
-        <v>0.2</v>
+        <v>0.48</v>
       </c>
       <c r="J14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1134,13 +1134,13 @@
         <v>2.5</v>
       </c>
       <c r="F15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="H15" s="1">
-        <v>0.2</v>
+        <v>0.48</v>
       </c>
       <c r="J15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1170,13 +1170,13 @@
         <v>2.5</v>
       </c>
       <c r="F16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" s="1">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="H16" s="1">
-        <v>0.2</v>
+        <v>0.48</v>
       </c>
       <c r="J16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1206,13 +1206,13 @@
         <v>2.5</v>
       </c>
       <c r="F17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="H17" s="1">
-        <v>0.2</v>
+        <v>0.48</v>
       </c>
       <c r="J17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1242,7 +1242,7 @@
         <v>2.5</v>
       </c>
       <c r="F18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="1">
         <v>0.1</v>
@@ -1278,7 +1278,7 @@
         <v>2.5</v>
       </c>
       <c r="F19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1">
         <v>0.1</v>
@@ -1314,7 +1314,7 @@
         <v>2.5</v>
       </c>
       <c r="F20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1">
         <v>0.1</v>
@@ -1350,13 +1350,13 @@
         <v>2.5</v>
       </c>
       <c r="F21" s="1">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="G21" s="1">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="H21" s="1">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="J21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1386,13 +1386,13 @@
         <v>2.5</v>
       </c>
       <c r="F22" s="1">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="G22" s="1">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="H22" s="1">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="J22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1422,13 +1422,13 @@
         <v>2.5</v>
       </c>
       <c r="F23" s="1">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="G23" s="1">
-        <v>0.1</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="H23" s="1">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="J23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1494,7 +1494,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1560,7 +1560,7 @@
         <v>2.5</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
         <v>0.1</v>
@@ -1596,7 +1596,7 @@
         <v>2.5</v>
       </c>
       <c r="F3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <v>0.1</v>
@@ -1632,7 +1632,7 @@
         <v>2.5</v>
       </c>
       <c r="F4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
         <v>0.1</v>
@@ -1668,7 +1668,7 @@
         <v>2.5</v>
       </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
         <v>0.1</v>
@@ -1704,7 +1704,7 @@
         <v>2.5</v>
       </c>
       <c r="F6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1">
         <v>0.1</v>
@@ -1740,7 +1740,7 @@
         <v>2.5</v>
       </c>
       <c r="F7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1">
         <v>0.1</v>
@@ -1776,7 +1776,7 @@
         <v>2.5</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
         <v>0.1</v>
@@ -1812,7 +1812,7 @@
         <v>2.5</v>
       </c>
       <c r="F9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1">
         <v>0.1</v>
@@ -1848,7 +1848,7 @@
         <v>2.5</v>
       </c>
       <c r="F10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1">
         <v>0.1</v>
@@ -1884,7 +1884,7 @@
         <v>2.5</v>
       </c>
       <c r="F11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
         <v>0.1</v>
@@ -1920,7 +1920,7 @@
         <v>2.5</v>
       </c>
       <c r="F12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1">
         <v>0.1</v>
@@ -1956,7 +1956,7 @@
         <v>2.5</v>
       </c>
       <c r="F13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1">
         <v>0.1</v>
@@ -1992,7 +1992,7 @@
         <v>2.5</v>
       </c>
       <c r="F14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1">
         <v>0.1</v>
@@ -2028,7 +2028,7 @@
         <v>2.5</v>
       </c>
       <c r="F15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1">
         <v>0.1</v>
@@ -2064,7 +2064,7 @@
         <v>2.5</v>
       </c>
       <c r="F16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" s="1">
         <v>0.1</v>
@@ -2100,7 +2100,7 @@
         <v>2.5</v>
       </c>
       <c r="F17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1">
         <v>0.1</v>
@@ -2136,7 +2136,7 @@
         <v>2.5</v>
       </c>
       <c r="F18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="1">
         <v>0.1</v>
@@ -2172,7 +2172,7 @@
         <v>2.5</v>
       </c>
       <c r="F19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1">
         <v>0.1</v>
@@ -2208,7 +2208,7 @@
         <v>2.5</v>
       </c>
       <c r="F20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1">
         <v>0.1</v>
@@ -2244,7 +2244,7 @@
         <v>2.5</v>
       </c>
       <c r="F21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="1">
         <v>0.1</v>
@@ -2280,7 +2280,7 @@
         <v>2.5</v>
       </c>
       <c r="F22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" s="1">
         <v>0.1</v>
@@ -2316,7 +2316,7 @@
         <v>2.5</v>
       </c>
       <c r="F23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23" s="1">
         <v>0.1</v>
@@ -2386,9 +2386,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F923A3F-B1CE-4620-BAAF-3B4B2F6906AC}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="F2" sqref="F2:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2455,7 +2455,7 @@
         <v>2.5</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
         <v>0.1</v>
@@ -2491,7 +2491,7 @@
         <v>2.5</v>
       </c>
       <c r="F3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
         <v>0.1</v>
@@ -2527,7 +2527,7 @@
         <v>2.5</v>
       </c>
       <c r="F4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
         <v>0.1</v>
@@ -2563,7 +2563,7 @@
         <v>2.5</v>
       </c>
       <c r="F5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
         <v>0.1</v>
@@ -2599,7 +2599,7 @@
         <v>2.5</v>
       </c>
       <c r="F6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1">
         <v>0.1</v>
@@ -2635,7 +2635,7 @@
         <v>2.5</v>
       </c>
       <c r="F7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1">
         <v>0.1</v>
@@ -2671,7 +2671,7 @@
         <v>2.5</v>
       </c>
       <c r="F8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
         <v>0.1</v>
@@ -2707,7 +2707,7 @@
         <v>2.5</v>
       </c>
       <c r="F9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" s="1">
         <v>0.1</v>
@@ -2743,7 +2743,7 @@
         <v>2.5</v>
       </c>
       <c r="F10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="1">
         <v>0.1</v>
@@ -2779,7 +2779,7 @@
         <v>2.5</v>
       </c>
       <c r="F11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
         <v>0.1</v>
@@ -2815,7 +2815,7 @@
         <v>2.5</v>
       </c>
       <c r="F12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G12" s="1">
         <v>0.1</v>
@@ -2851,7 +2851,7 @@
         <v>2.5</v>
       </c>
       <c r="F13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13" s="1">
         <v>0.1</v>
@@ -2887,7 +2887,7 @@
         <v>2.5</v>
       </c>
       <c r="F14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1">
         <v>0.1</v>
@@ -2923,7 +2923,7 @@
         <v>2.5</v>
       </c>
       <c r="F15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1">
         <v>0.1</v>
@@ -2959,7 +2959,7 @@
         <v>2.5</v>
       </c>
       <c r="F16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" s="1">
         <v>0.1</v>
@@ -2995,7 +2995,7 @@
         <v>2.5</v>
       </c>
       <c r="F17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1">
         <v>0.1</v>
@@ -3031,7 +3031,7 @@
         <v>2.5</v>
       </c>
       <c r="F18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G18" s="1">
         <v>0.1</v>
@@ -3067,7 +3067,7 @@
         <v>2.5</v>
       </c>
       <c r="F19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1">
         <v>0.1</v>
@@ -3103,7 +3103,7 @@
         <v>2.5</v>
       </c>
       <c r="F20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1">
         <v>0.1</v>
@@ -3139,7 +3139,7 @@
         <v>2.5</v>
       </c>
       <c r="F21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21" s="1">
         <v>0.1</v>
@@ -3175,7 +3175,7 @@
         <v>2.5</v>
       </c>
       <c r="F22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22" s="1">
         <v>0.1</v>
@@ -3211,7 +3211,7 @@
         <v>2.5</v>
       </c>
       <c r="F23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23" s="1">
         <v>0.1</v>
@@ -3247,7 +3247,7 @@
         <v>2.5</v>
       </c>
       <c r="F24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1">
         <v>0.1</v>
@@ -3283,7 +3283,7 @@
         <v>2.5</v>
       </c>
       <c r="F25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25" s="1">
         <v>0.1</v>

</xml_diff>

<commit_message>
Water Tower Design Base
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Tower.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Tower.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F1D0FB-62B3-42BE-882F-8835D6E69BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C108518-F8BF-49F7-856A-1D3BA93E45DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4575" windowWidth="29040" windowHeight="15840" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-19650" yWindow="5805" windowWidth="19425" windowHeight="12165" activeTab="1" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="FIRE" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="65">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -262,6 +262,37 @@
   </si>
   <si>
     <t>projspf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.2;0.8;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.2;0.9;</t>
+  </si>
+  <si>
+    <t>0.3;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.1;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.5;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.4;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.6;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0.2;0.8;1.4;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -631,9 +662,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53B544D-229D-4A5B-BFF8-79DA3F65400C}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
+      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1527,7 +1558,7 @@
         <v>2.5</v>
       </c>
       <c r="F21" s="1">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="G21" s="1">
         <v>7.4999999999999997E-2</v>
@@ -1572,7 +1603,7 @@
         <v>2.5</v>
       </c>
       <c r="F22" s="1">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="G22" s="1">
         <v>7.4999999999999997E-2</v>
@@ -1617,7 +1648,7 @@
         <v>2.5</v>
       </c>
       <c r="F23" s="1">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="G23" s="1">
         <v>7.4999999999999997E-2</v>
@@ -1696,9 +1727,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE2B3F2-784A-4749-859E-0B1CD32F0B4D}">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1773,13 +1804,13 @@
         <v>2.5</v>
       </c>
       <c r="F2" s="1">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="G2" s="1">
         <v>0.1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="I2" s="1">
         <v>0</v>
@@ -1812,13 +1843,13 @@
         <v>2.5</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="G3" s="1">
         <v>0.1</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="I3" s="1">
         <v>0</v>
@@ -1857,7 +1888,7 @@
         <v>0.1</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="I4" s="1">
         <v>0</v>
@@ -1896,10 +1927,16 @@
         <v>0.1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.3</v>
       </c>
       <c r="M5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1935,10 +1972,16 @@
         <v>0.1</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.3</v>
       </c>
       <c r="M6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1974,7 +2017,7 @@
         <v>0.1</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -2013,7 +2056,7 @@
         <v>0.1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="I8" s="1">
         <v>0</v>
@@ -2052,7 +2095,7 @@
         <v>0.1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="I9" s="1">
         <v>0</v>
@@ -2091,10 +2134,16 @@
         <v>0.1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.3</v>
       </c>
       <c r="M10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2130,10 +2179,16 @@
         <v>0.1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="I11" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.3</v>
       </c>
       <c r="M11" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2169,10 +2224,16 @@
         <v>0.1</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="I12" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.3</v>
       </c>
       <c r="M12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2208,7 +2269,7 @@
         <v>0.1</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="I13" s="1">
         <v>0</v>
@@ -2247,7 +2308,7 @@
         <v>0.1</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="I14" s="1">
         <v>0</v>
@@ -2286,10 +2347,16 @@
         <v>0.1</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="I15" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.3</v>
       </c>
       <c r="M15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2325,10 +2392,16 @@
         <v>0.1</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.3</v>
       </c>
       <c r="M16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2364,10 +2437,16 @@
         <v>0.1</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="I17" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.3</v>
       </c>
       <c r="M17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2403,10 +2482,16 @@
         <v>0.1</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="I18" s="1">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.45</v>
       </c>
       <c r="M18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2442,10 +2527,16 @@
         <v>0.1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="I19" s="1">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.45</v>
       </c>
       <c r="M19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2481,10 +2572,16 @@
         <v>0.1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="I20" s="1">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.45</v>
       </c>
       <c r="M20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2520,10 +2617,16 @@
         <v>0.1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="I21" s="1">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.45</v>
       </c>
       <c r="M21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2553,16 +2656,22 @@
         <v>2.5</v>
       </c>
       <c r="F22" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G22" s="1">
         <v>0.1</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="I22" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.3</v>
       </c>
       <c r="M22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2592,16 +2701,22 @@
         <v>2.5</v>
       </c>
       <c r="F23" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G23" s="1">
         <v>0.1</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="I23" s="1">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.3</v>
       </c>
       <c r="M23" s="1" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Water Tower Effect Base
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Tower.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Tower.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4BAE1B-1A26-48D3-B376-295A4CBD2DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF94A1B-8F75-489A-A5D2-1AAEF324EFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4575" windowWidth="29040" windowHeight="15840" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-19755" yWindow="5745" windowWidth="19425" windowHeight="12165" activeTab="1" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="FIRE" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="80">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -331,6 +331,21 @@
   </si>
   <si>
     <t>(1,0,0,1)</t>
+  </si>
+  <si>
+    <t>(1,0,0,1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선장,Captain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(0.6,0.8,1,1)</t>
+  </si>
+  <si>
+    <t>(0.6,0.8,1,1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>(1,0,0,1)</t>
@@ -703,9 +718,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E53B544D-229D-4A5B-BFF8-79DA3F65400C}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V6" sqref="V6"/>
+      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1865,9 +1880,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE2B3F2-784A-4749-859E-0B1CD32F0B4D}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2106,7 +2121,7 @@
         <v>1012001</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1">
         <v>150</v>
@@ -2137,6 +2152,12 @@
       </c>
       <c r="L6" s="1">
         <v>0.3</v>
+      </c>
+      <c r="M6" s="1">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="P6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2177,6 +2198,9 @@
       <c r="I7" s="1">
         <v>0</v>
       </c>
+      <c r="N7" t="s">
+        <v>77</v>
+      </c>
       <c r="P7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1010002/</v>
@@ -2216,6 +2240,9 @@
       <c r="I8" s="1">
         <v>0</v>
       </c>
+      <c r="N8" t="s">
+        <v>77</v>
+      </c>
       <c r="P8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1011002/</v>
@@ -2255,6 +2282,9 @@
       <c r="I9" s="1">
         <v>0</v>
       </c>
+      <c r="N9" t="s">
+        <v>77</v>
+      </c>
       <c r="P9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1012002/</v>
@@ -2303,6 +2333,9 @@
       <c r="L10" s="1">
         <v>0.3</v>
       </c>
+      <c r="N10" t="s">
+        <v>77</v>
+      </c>
       <c r="P10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1010003/</v>
@@ -2351,6 +2384,9 @@
       <c r="L11" s="1">
         <v>0.3</v>
       </c>
+      <c r="N11" t="s">
+        <v>77</v>
+      </c>
       <c r="P11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1011003/</v>
@@ -2399,6 +2435,9 @@
       <c r="L12" s="1">
         <v>0.3</v>
       </c>
+      <c r="N12" t="s">
+        <v>77</v>
+      </c>
       <c r="P12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1012003/</v>
@@ -2438,6 +2477,9 @@
       <c r="I13" s="1">
         <v>0</v>
       </c>
+      <c r="N13" t="s">
+        <v>77</v>
+      </c>
       <c r="P13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1011004/</v>
@@ -2477,6 +2519,9 @@
       <c r="I14" s="1">
         <v>0</v>
       </c>
+      <c r="N14" t="s">
+        <v>77</v>
+      </c>
       <c r="P14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1012004/</v>
@@ -2525,6 +2570,9 @@
       <c r="L15" s="1">
         <v>0.3</v>
       </c>
+      <c r="N15" t="s">
+        <v>77</v>
+      </c>
       <c r="P15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1010005/</v>
@@ -2573,6 +2621,9 @@
       <c r="L16" s="1">
         <v>0.3</v>
       </c>
+      <c r="N16" t="s">
+        <v>77</v>
+      </c>
       <c r="P16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1011005/</v>
@@ -2621,6 +2672,9 @@
       <c r="L17" s="1">
         <v>0.3</v>
       </c>
+      <c r="N17" t="s">
+        <v>77</v>
+      </c>
       <c r="P17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1012005/</v>
@@ -2669,6 +2723,9 @@
       <c r="L18" s="1">
         <v>0.15</v>
       </c>
+      <c r="N18" t="s">
+        <v>78</v>
+      </c>
       <c r="P18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1010006/</v>
@@ -2717,6 +2774,9 @@
       <c r="L19" s="1">
         <v>0.15</v>
       </c>
+      <c r="N19" t="s">
+        <v>78</v>
+      </c>
       <c r="P19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1011006/</v>
@@ -2765,6 +2825,9 @@
       <c r="L20" s="1">
         <v>0.15</v>
       </c>
+      <c r="N20" t="s">
+        <v>77</v>
+      </c>
       <c r="P20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1012006/</v>
@@ -2813,6 +2876,9 @@
       <c r="L21" s="1">
         <v>0.15</v>
       </c>
+      <c r="N21" t="s">
+        <v>77</v>
+      </c>
       <c r="P21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1013006/</v>
@@ -2861,6 +2927,12 @@
       <c r="L22" s="1">
         <v>0.3</v>
       </c>
+      <c r="M22" s="1">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="P22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1012007/</v>
@@ -2908,6 +2980,12 @@
       </c>
       <c r="L23" s="1">
         <v>0.3</v>
+      </c>
+      <c r="M23" s="1">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="P23" s="1" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Nature Tower Effect Base
</commit_message>
<xml_diff>
--- a/Utils/Excel To Json/bin/netcoreapp3.1/Tower.xlsx
+++ b/Utils/Excel To Json/bin/netcoreapp3.1/Tower.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Unity\TETD\Utils\Excel To Json\bin\netcoreapp3.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF94A1B-8F75-489A-A5D2-1AAEF324EFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EC2AAE-7E35-4FA3-B515-913D8C174DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19755" yWindow="5745" windowWidth="19425" windowHeight="12165" activeTab="1" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
+    <workbookView xWindow="-19755" yWindow="5745" windowWidth="19425" windowHeight="12165" activeTab="2" xr2:uid="{F7863118-105F-453F-BD22-09F23552EC2F}"/>
   </bookViews>
   <sheets>
     <sheet name="FIRE" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="81">
   <si>
     <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -349,6 +349,10 @@
   </si>
   <si>
     <t>(1,0,0,1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(1,0,1,1)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1880,7 +1884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE2B3F2-784A-4749-859E-0B1CD32F0B4D}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
     </sheetView>
@@ -3049,9 +3053,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F923A3F-B1CE-4620-BAAF-3B4B2F6906AC}">
   <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1:O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3160,6 +3164,9 @@
       <c r="L2" s="1">
         <v>0.3</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="P2" s="1" t="str">
         <f t="shared" ref="P2:P25" si="0">CONCATENATE("/Sprites/Tower/",A2,"/")</f>
         <v>/Sprites/Tower/1020000/</v>
@@ -3208,6 +3215,9 @@
       <c r="L3" s="1">
         <v>0.3</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="P3" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1021000/</v>
@@ -3544,6 +3554,9 @@
       <c r="L10" s="1">
         <v>0.3</v>
       </c>
+      <c r="N10" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="P10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1020003/</v>
@@ -3592,6 +3605,9 @@
       <c r="L11" s="1">
         <v>0.3</v>
       </c>
+      <c r="N11" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="P11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>/Sprites/Tower/1021003/</v>
@@ -3639,6 +3655,9 @@
       </c>
       <c r="L12" s="1">
         <v>0.3</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="P12" s="1" t="str">
         <f t="shared" si="0"/>

</xml_diff>